<commit_message>
adding background color changer to the header
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -281,7 +281,7 @@
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -298,6 +298,11 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,7 +481,7 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -768,7 +773,7 @@
     <xf numFmtId="168" fontId="36" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="41" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -816,6 +821,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="38" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -4020,69 +4028,69 @@
       <c r="B20" s="65" t="n"/>
     </row>
     <row r="21" ht="27" customHeight="1">
-      <c r="A21" s="120" t="inlineStr">
+      <c r="A21" s="129" t="inlineStr">
         <is>
           <t>Mark &amp; Nº</t>
         </is>
       </c>
-      <c r="B21" s="120" t="inlineStr">
+      <c r="B21" s="129" t="inlineStr">
         <is>
           <t>P.O N°</t>
         </is>
       </c>
-      <c r="C21" s="120" t="inlineStr">
+      <c r="C21" s="129" t="inlineStr">
         <is>
           <t>ITEM N°</t>
         </is>
       </c>
-      <c r="D21" s="120" t="inlineStr">
+      <c r="D21" s="129" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E21" s="120" t="inlineStr">
+      <c r="E21" s="129" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="F21" s="129" t="n"/>
-      <c r="G21" s="120" t="inlineStr">
+      <c r="F21" s="130" t="n"/>
+      <c r="G21" s="129" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
         </is>
       </c>
-      <c r="H21" s="120" t="inlineStr">
+      <c r="H21" s="129" t="inlineStr">
         <is>
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="120" t="inlineStr">
+      <c r="I21" s="129" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="130" t="n"/>
-      <c r="B22" s="130" t="n"/>
-      <c r="C22" s="130" t="n"/>
-      <c r="D22" s="130" t="n"/>
-      <c r="E22" s="120" t="inlineStr">
+      <c r="A22" s="131" t="n"/>
+      <c r="B22" s="131" t="n"/>
+      <c r="C22" s="131" t="n"/>
+      <c r="D22" s="131" t="n"/>
+      <c r="E22" s="129" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
       </c>
-      <c r="F22" s="120" t="inlineStr">
+      <c r="F22" s="129" t="inlineStr">
         <is>
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="130" t="n"/>
-      <c r="H22" s="130" t="n"/>
-      <c r="I22" s="130" t="n"/>
+      <c r="G22" s="131" t="n"/>
+      <c r="H22" s="131" t="n"/>
+      <c r="I22" s="131" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
-      <c r="A23" s="131" t="inlineStr">
+      <c r="A23" s="132" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
@@ -4096,7 +4104,7 @@
         </is>
       </c>
       <c r="D23" s="111" t="n"/>
-      <c r="E23" s="132" t="n">
+      <c r="E23" s="133" t="n">
         <v>83</v>
       </c>
       <c r="F23" s="123" t="n">
@@ -4108,12 +4116,12 @@
       <c r="H23" s="123" t="n">
         <v>435.75</v>
       </c>
-      <c r="I23" s="133" t="n">
+      <c r="I23" s="134" t="n">
         <v>1.4686</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="134" t="inlineStr">
+      <c r="A24" s="135" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
@@ -4127,7 +4135,7 @@
         </is>
       </c>
       <c r="D24" s="111" t="n"/>
-      <c r="E24" s="132" t="n">
+      <c r="E24" s="133" t="n">
         <v>5</v>
       </c>
       <c r="F24" s="123" t="n">
@@ -4139,12 +4147,12 @@
       <c r="H24" s="123" t="n">
         <v>26.25</v>
       </c>
-      <c r="I24" s="133" t="n">
+      <c r="I24" s="134" t="n">
         <v>0.0885</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="134" t="inlineStr">
+      <c r="A25" s="135" t="inlineStr">
         <is>
           <t>Case Qty:</t>
         </is>
@@ -4158,7 +4166,7 @@
         </is>
       </c>
       <c r="D25" s="111" t="n"/>
-      <c r="E25" s="132" t="n">
+      <c r="E25" s="133" t="n">
         <v>6</v>
       </c>
       <c r="F25" s="123" t="n">
@@ -4170,12 +4178,12 @@
       <c r="H25" s="123" t="n">
         <v>31.5</v>
       </c>
-      <c r="I25" s="133" t="n">
+      <c r="I25" s="134" t="n">
         <v>0.1062</v>
       </c>
     </row>
     <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="134" t="inlineStr">
+      <c r="A26" s="135" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
@@ -4189,7 +4197,7 @@
         </is>
       </c>
       <c r="D26" s="111" t="n"/>
-      <c r="E26" s="132" t="n">
+      <c r="E26" s="133" t="n">
         <v>101</v>
       </c>
       <c r="F26" s="123" t="n">
@@ -4201,12 +4209,12 @@
       <c r="H26" s="123" t="n">
         <v>453.0972</v>
       </c>
-      <c r="I26" s="133" t="n">
+      <c r="I26" s="134" t="n">
         <v>1.5554</v>
       </c>
     </row>
     <row r="27" ht="27" customHeight="1">
-      <c r="A27" s="135" t="n"/>
+      <c r="A27" s="136" t="n"/>
       <c r="B27" s="122" t="n">
         <v>9000637260</v>
       </c>
@@ -4216,7 +4224,7 @@
         </is>
       </c>
       <c r="D27" s="111" t="n"/>
-      <c r="E27" s="132" t="n">
+      <c r="E27" s="133" t="n">
         <v>7</v>
       </c>
       <c r="F27" s="123" t="n">
@@ -4228,12 +4236,12 @@
       <c r="H27" s="123" t="n">
         <v>31.4028</v>
       </c>
-      <c r="I27" s="133" t="n">
+      <c r="I27" s="134" t="n">
         <v>0.1078</v>
       </c>
     </row>
     <row r="28" ht="27" customHeight="1">
-      <c r="A28" s="135" t="n"/>
+      <c r="A28" s="136" t="n"/>
       <c r="B28" s="122" t="n">
         <v>9000619872</v>
       </c>
@@ -4243,7 +4251,7 @@
         </is>
       </c>
       <c r="D28" s="111" t="n"/>
-      <c r="E28" s="132" t="n">
+      <c r="E28" s="133" t="n">
         <v>135</v>
       </c>
       <c r="F28" s="123" t="n">
@@ -4255,12 +4263,12 @@
       <c r="H28" s="123" t="n">
         <v>612</v>
       </c>
-      <c r="I28" s="133" t="n">
+      <c r="I28" s="134" t="n">
         <v>1.9008</v>
       </c>
     </row>
     <row r="29" ht="27" customHeight="1">
-      <c r="A29" s="135" t="n"/>
+      <c r="A29" s="136" t="n"/>
       <c r="B29" s="122" t="n">
         <v>9000619872</v>
       </c>
@@ -4270,7 +4278,7 @@
         </is>
       </c>
       <c r="D29" s="111" t="n"/>
-      <c r="E29" s="132" t="n">
+      <c r="E29" s="133" t="n">
         <v>109</v>
       </c>
       <c r="F29" s="123" t="n">
@@ -4282,12 +4290,12 @@
       <c r="H29" s="123" t="n">
         <v>500.7188</v>
       </c>
-      <c r="I29" s="133" t="n">
+      <c r="I29" s="134" t="n">
         <v>1.9655</v>
       </c>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="135" t="n"/>
+      <c r="A30" s="136" t="n"/>
       <c r="B30" s="122" t="n">
         <v>9000619872</v>
       </c>
@@ -4297,7 +4305,7 @@
         </is>
       </c>
       <c r="D30" s="111" t="n"/>
-      <c r="E30" s="132" t="n">
+      <c r="E30" s="133" t="n">
         <v>3</v>
       </c>
       <c r="F30" s="123" t="n">
@@ -4309,12 +4317,12 @@
       <c r="H30" s="123" t="n">
         <v>13.7813</v>
       </c>
-      <c r="I30" s="133" t="n">
+      <c r="I30" s="134" t="n">
         <v>0.0541</v>
       </c>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="A31" s="135" t="n"/>
+      <c r="A31" s="136" t="n"/>
       <c r="B31" s="122" t="n">
         <v>9000619872</v>
       </c>
@@ -4324,7 +4332,7 @@
         </is>
       </c>
       <c r="D31" s="111" t="n"/>
-      <c r="E31" s="132" t="n">
+      <c r="E31" s="133" t="n">
         <v>27</v>
       </c>
       <c r="F31" s="123" t="n">
@@ -4336,12 +4344,12 @@
       <c r="H31" s="123" t="n">
         <v>159</v>
       </c>
-      <c r="I31" s="133" t="n">
+      <c r="I31" s="134" t="n">
         <v>2.772</v>
       </c>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="135" t="n"/>
+      <c r="A32" s="136" t="n"/>
       <c r="B32" s="122" t="n">
         <v>9000661047</v>
       </c>
@@ -4351,7 +4359,7 @@
         </is>
       </c>
       <c r="D32" s="111" t="n"/>
-      <c r="E32" s="132" t="n">
+      <c r="E32" s="133" t="n">
         <v>226</v>
       </c>
       <c r="F32" s="123" t="n">
@@ -4363,12 +4371,12 @@
       <c r="H32" s="123" t="n">
         <v>989.7076</v>
       </c>
-      <c r="I32" s="133" t="n">
+      <c r="I32" s="134" t="n">
         <v>2.8062</v>
       </c>
     </row>
     <row r="33" ht="27" customHeight="1">
-      <c r="A33" s="135" t="n"/>
+      <c r="A33" s="136" t="n"/>
       <c r="B33" s="122" t="n">
         <v>9000661047</v>
       </c>
@@ -4378,7 +4386,7 @@
         </is>
       </c>
       <c r="D33" s="111" t="n"/>
-      <c r="E33" s="132" t="n">
+      <c r="E33" s="133" t="n">
         <v>10</v>
       </c>
       <c r="F33" s="123" t="n">
@@ -4390,12 +4398,12 @@
       <c r="H33" s="123" t="n">
         <v>43.7924</v>
       </c>
-      <c r="I33" s="133" t="n">
+      <c r="I33" s="134" t="n">
         <v>0.1242</v>
       </c>
     </row>
     <row r="34" ht="27" customHeight="1">
-      <c r="A34" s="135" t="n"/>
+      <c r="A34" s="136" t="n"/>
       <c r="B34" s="122" t="n">
         <v>9000632447</v>
       </c>
@@ -4405,7 +4413,7 @@
         </is>
       </c>
       <c r="D34" s="111" t="n"/>
-      <c r="E34" s="132" t="n">
+      <c r="E34" s="133" t="n">
         <v>146</v>
       </c>
       <c r="F34" s="123" t="n">
@@ -4417,12 +4425,12 @@
       <c r="H34" s="123" t="n">
         <v>868.6014</v>
       </c>
-      <c r="I34" s="133" t="n">
+      <c r="I34" s="134" t="n">
         <v>2.4611</v>
       </c>
     </row>
     <row r="35" ht="27" customHeight="1">
-      <c r="A35" s="135" t="n"/>
+      <c r="A35" s="136" t="n"/>
       <c r="B35" s="122" t="n">
         <v>9000632447</v>
       </c>
@@ -4432,7 +4440,7 @@
         </is>
       </c>
       <c r="D35" s="111" t="n"/>
-      <c r="E35" s="132" t="n">
+      <c r="E35" s="133" t="n">
         <v>2</v>
       </c>
       <c r="F35" s="123" t="n">
@@ -4444,12 +4452,12 @@
       <c r="H35" s="123" t="n">
         <v>11.8986</v>
       </c>
-      <c r="I35" s="133" t="n">
+      <c r="I35" s="134" t="n">
         <v>0.0337</v>
       </c>
     </row>
     <row r="36" ht="27" customHeight="1">
-      <c r="A36" s="135" t="n"/>
+      <c r="A36" s="136" t="n"/>
       <c r="B36" s="122" t="n">
         <v>9000591002</v>
       </c>
@@ -4459,7 +4467,7 @@
         </is>
       </c>
       <c r="D36" s="111" t="n"/>
-      <c r="E36" s="132" t="n">
+      <c r="E36" s="133" t="n">
         <v>210</v>
       </c>
       <c r="F36" s="123" t="n">
@@ -4471,12 +4479,12 @@
       <c r="H36" s="123" t="n">
         <v>866.7453</v>
       </c>
-      <c r="I36" s="133" t="n">
+      <c r="I36" s="134" t="n">
         <v>2.7458</v>
       </c>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="A37" s="135" t="n"/>
+      <c r="A37" s="136" t="n"/>
       <c r="B37" s="122" t="n">
         <v>9000591002</v>
       </c>
@@ -4486,7 +4494,7 @@
         </is>
       </c>
       <c r="D37" s="111" t="n"/>
-      <c r="E37" s="132" t="n">
+      <c r="E37" s="133" t="n">
         <v>2</v>
       </c>
       <c r="F37" s="123" t="n">
@@ -4498,12 +4506,12 @@
       <c r="H37" s="123" t="n">
         <v>8.2547</v>
       </c>
-      <c r="I37" s="133" t="n">
+      <c r="I37" s="134" t="n">
         <v>0.0262</v>
       </c>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="A38" s="135" t="n"/>
+      <c r="A38" s="136" t="n"/>
       <c r="B38" s="122" t="n">
         <v>9000591002</v>
       </c>
@@ -4513,7 +4521,7 @@
         </is>
       </c>
       <c r="D38" s="111" t="n"/>
-      <c r="E38" s="132" t="n">
+      <c r="E38" s="133" t="n">
         <v>128</v>
       </c>
       <c r="F38" s="123" t="n">
@@ -4525,12 +4533,12 @@
       <c r="H38" s="123" t="n">
         <v>513.4884</v>
       </c>
-      <c r="I38" s="133" t="n">
+      <c r="I38" s="134" t="n">
         <v>1.6896</v>
       </c>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="A39" s="135" t="n"/>
+      <c r="A39" s="136" t="n"/>
       <c r="B39" s="122" t="n">
         <v>9000591002</v>
       </c>
@@ -4540,7 +4548,7 @@
         </is>
       </c>
       <c r="D39" s="111" t="n"/>
-      <c r="E39" s="132" t="n">
+      <c r="E39" s="133" t="n">
         <v>1</v>
       </c>
       <c r="F39" s="123" t="n">
@@ -4552,12 +4560,12 @@
       <c r="H39" s="123" t="n">
         <v>4.0116</v>
       </c>
-      <c r="I39" s="133" t="n">
+      <c r="I39" s="134" t="n">
         <v>0.0132</v>
       </c>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="A40" s="135" t="n"/>
+      <c r="A40" s="136" t="n"/>
       <c r="B40" s="122" t="n">
         <v>9000663929</v>
       </c>
@@ -4567,7 +4575,7 @@
         </is>
       </c>
       <c r="D40" s="111" t="n"/>
-      <c r="E40" s="132" t="n">
+      <c r="E40" s="133" t="n">
         <v>101</v>
       </c>
       <c r="F40" s="123" t="n">
@@ -4579,12 +4587,12 @@
       <c r="H40" s="123" t="n">
         <v>492.375</v>
       </c>
-      <c r="I40" s="133" t="n">
+      <c r="I40" s="134" t="n">
         <v>1.7306</v>
       </c>
     </row>
     <row r="41" ht="27" customHeight="1">
-      <c r="A41" s="135" t="n"/>
+      <c r="A41" s="136" t="n"/>
       <c r="B41" s="122" t="n">
         <v>9000663929</v>
       </c>
@@ -4594,7 +4602,7 @@
         </is>
       </c>
       <c r="D41" s="111" t="n"/>
-      <c r="E41" s="132" t="n">
+      <c r="E41" s="133" t="n">
         <v>3</v>
       </c>
       <c r="F41" s="123" t="n">
@@ -4606,12 +4614,12 @@
       <c r="H41" s="123" t="n">
         <v>14.625</v>
       </c>
-      <c r="I41" s="133" t="n">
+      <c r="I41" s="134" t="n">
         <v>0.0514</v>
       </c>
     </row>
     <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="135" t="n"/>
+      <c r="A42" s="136" t="n"/>
       <c r="B42" s="122" t="n">
         <v>9000653386</v>
       </c>
@@ -4621,7 +4629,7 @@
         </is>
       </c>
       <c r="D42" s="111" t="n"/>
-      <c r="E42" s="132" t="n">
+      <c r="E42" s="133" t="n">
         <v>134</v>
       </c>
       <c r="F42" s="123" t="n">
@@ -4633,12 +4641,12 @@
       <c r="H42" s="123" t="n">
         <v>392.0213</v>
       </c>
-      <c r="I42" s="133" t="n">
+      <c r="I42" s="134" t="n">
         <v>1.5054</v>
       </c>
     </row>
     <row r="43" ht="27" customHeight="1">
-      <c r="A43" s="135" t="n"/>
+      <c r="A43" s="136" t="n"/>
       <c r="B43" s="122" t="n">
         <v>9000653386</v>
       </c>
@@ -4648,7 +4656,7 @@
         </is>
       </c>
       <c r="D43" s="111" t="n"/>
-      <c r="E43" s="132" t="n">
+      <c r="E43" s="133" t="n">
         <v>7</v>
       </c>
       <c r="F43" s="123" t="n">
@@ -4660,12 +4668,12 @@
       <c r="H43" s="123" t="n">
         <v>20.4787</v>
       </c>
-      <c r="I43" s="133" t="n">
+      <c r="I43" s="134" t="n">
         <v>0.0786</v>
       </c>
     </row>
     <row r="44" ht="27" customHeight="1">
-      <c r="A44" s="135" t="n"/>
+      <c r="A44" s="136" t="n"/>
       <c r="B44" s="122" t="n">
         <v>9000689724</v>
       </c>
@@ -4675,7 +4683,7 @@
         </is>
       </c>
       <c r="D44" s="111" t="n"/>
-      <c r="E44" s="132" t="n">
+      <c r="E44" s="133" t="n">
         <v>182</v>
       </c>
       <c r="F44" s="123" t="n">
@@ -4687,12 +4695,12 @@
       <c r="H44" s="123" t="n">
         <v>782.3214</v>
       </c>
-      <c r="I44" s="133" t="n">
+      <c r="I44" s="134" t="n">
         <v>2.2063</v>
       </c>
     </row>
     <row r="45" ht="27" customHeight="1">
-      <c r="A45" s="135" t="n"/>
+      <c r="A45" s="136" t="n"/>
       <c r="B45" s="122" t="n">
         <v>9000689724</v>
       </c>
@@ -4702,7 +4710,7 @@
         </is>
       </c>
       <c r="D45" s="111" t="n"/>
-      <c r="E45" s="132" t="n">
+      <c r="E45" s="133" t="n">
         <v>14</v>
       </c>
       <c r="F45" s="123" t="n">
@@ -4714,12 +4722,12 @@
       <c r="H45" s="123" t="n">
         <v>60.1786</v>
       </c>
-      <c r="I45" s="133" t="n">
+      <c r="I45" s="134" t="n">
         <v>0.1697</v>
       </c>
     </row>
     <row r="46" ht="27" customHeight="1">
-      <c r="A46" s="135" t="n"/>
+      <c r="A46" s="136" t="n"/>
       <c r="B46" s="122" t="n">
         <v>9000689724</v>
       </c>
@@ -4729,7 +4737,7 @@
         </is>
       </c>
       <c r="D46" s="111" t="n"/>
-      <c r="E46" s="132" t="n">
+      <c r="E46" s="133" t="n">
         <v>203</v>
       </c>
       <c r="F46" s="123" t="n">
@@ -4741,12 +4749,12 @@
       <c r="H46" s="123" t="n">
         <v>842.2863</v>
       </c>
-      <c r="I46" s="133" t="n">
+      <c r="I46" s="134" t="n">
         <v>2.2042</v>
       </c>
     </row>
     <row r="47" ht="27" customHeight="1">
-      <c r="A47" s="135" t="n"/>
+      <c r="A47" s="136" t="n"/>
       <c r="B47" s="122" t="n">
         <v>9000689724</v>
       </c>
@@ -4756,7 +4764,7 @@
         </is>
       </c>
       <c r="D47" s="111" t="n"/>
-      <c r="E47" s="132" t="n">
+      <c r="E47" s="133" t="n">
         <v>29</v>
       </c>
       <c r="F47" s="123" t="n">
@@ -4768,12 +4776,12 @@
       <c r="H47" s="123" t="n">
         <v>120.3266</v>
       </c>
-      <c r="I47" s="133" t="n">
+      <c r="I47" s="134" t="n">
         <v>0.3149</v>
       </c>
     </row>
     <row r="48" ht="27" customHeight="1">
-      <c r="A48" s="135" t="n"/>
+      <c r="A48" s="136" t="n"/>
       <c r="B48" s="122" t="n">
         <v>9000689724</v>
       </c>
@@ -4783,7 +4791,7 @@
         </is>
       </c>
       <c r="D48" s="111" t="n"/>
-      <c r="E48" s="132" t="n">
+      <c r="E48" s="133" t="n">
         <v>16</v>
       </c>
       <c r="F48" s="123" t="n">
@@ -4795,12 +4803,12 @@
       <c r="H48" s="123" t="n">
         <v>66.3871</v>
       </c>
-      <c r="I48" s="133" t="n">
+      <c r="I48" s="134" t="n">
         <v>0.1737</v>
       </c>
     </row>
     <row r="49" ht="27" customHeight="1">
-      <c r="A49" s="135" t="n"/>
+      <c r="A49" s="136" t="n"/>
       <c r="B49" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4810,7 +4818,7 @@
         </is>
       </c>
       <c r="D49" s="111" t="n"/>
-      <c r="E49" s="132" t="n">
+      <c r="E49" s="133" t="n">
         <v>200</v>
       </c>
       <c r="F49" s="123" t="n">
@@ -4822,12 +4830,12 @@
       <c r="H49" s="123" t="n">
         <v>865</v>
       </c>
-      <c r="I49" s="133" t="n">
+      <c r="I49" s="134" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="50" ht="27" customHeight="1">
-      <c r="A50" s="135" t="n"/>
+      <c r="A50" s="136" t="n"/>
       <c r="B50" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4837,7 +4845,7 @@
         </is>
       </c>
       <c r="D50" s="111" t="n"/>
-      <c r="E50" s="132" t="n">
+      <c r="E50" s="133" t="n">
         <v>200</v>
       </c>
       <c r="F50" s="123" t="n">
@@ -4849,12 +4857,12 @@
       <c r="H50" s="123" t="n">
         <v>875.5</v>
       </c>
-      <c r="I50" s="133" t="n">
+      <c r="I50" s="134" t="n">
         <v>2.2572</v>
       </c>
     </row>
     <row r="51" ht="27" customHeight="1">
-      <c r="A51" s="135" t="n"/>
+      <c r="A51" s="136" t="n"/>
       <c r="B51" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4864,7 +4872,7 @@
         </is>
       </c>
       <c r="D51" s="111" t="n"/>
-      <c r="E51" s="132" t="n">
+      <c r="E51" s="133" t="n">
         <v>209</v>
       </c>
       <c r="F51" s="123" t="n">
@@ -4876,12 +4884,12 @@
       <c r="H51" s="123" t="n">
         <v>914</v>
       </c>
-      <c r="I51" s="133" t="n">
+      <c r="I51" s="134" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="52" ht="27" customHeight="1">
-      <c r="A52" s="135" t="n"/>
+      <c r="A52" s="136" t="n"/>
       <c r="B52" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4891,7 +4899,7 @@
         </is>
       </c>
       <c r="D52" s="111" t="n"/>
-      <c r="E52" s="132" t="n">
+      <c r="E52" s="133" t="n">
         <v>184</v>
       </c>
       <c r="F52" s="123" t="n">
@@ -4903,12 +4911,12 @@
       <c r="H52" s="123" t="n">
         <v>770.9259</v>
       </c>
-      <c r="I52" s="133" t="n">
+      <c r="I52" s="134" t="n">
         <v>2.2601</v>
       </c>
     </row>
     <row r="53" ht="27" customHeight="1">
-      <c r="A53" s="135" t="n"/>
+      <c r="A53" s="136" t="n"/>
       <c r="B53" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4918,7 +4926,7 @@
         </is>
       </c>
       <c r="D53" s="111" t="n"/>
-      <c r="E53" s="132" t="n">
+      <c r="E53" s="133" t="n">
         <v>32</v>
       </c>
       <c r="F53" s="123" t="n">
@@ -4930,12 +4938,12 @@
       <c r="H53" s="123" t="n">
         <v>134.0741</v>
       </c>
-      <c r="I53" s="133" t="n">
+      <c r="I53" s="134" t="n">
         <v>0.3931</v>
       </c>
     </row>
     <row r="54" ht="27" customFormat="1" customHeight="1" s="1">
-      <c r="A54" s="135" t="n"/>
+      <c r="A54" s="136" t="n"/>
       <c r="B54" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4945,7 +4953,7 @@
         </is>
       </c>
       <c r="D54" s="111" t="n"/>
-      <c r="E54" s="132" t="n">
+      <c r="E54" s="133" t="n">
         <v>177</v>
       </c>
       <c r="F54" s="123" t="n">
@@ -4957,12 +4965,12 @@
       <c r="H54" s="123" t="n">
         <v>764.8262999999999</v>
       </c>
-      <c r="I54" s="133" t="n">
+      <c r="I54" s="134" t="n">
         <v>2.4717</v>
       </c>
     </row>
     <row r="55" ht="27" customHeight="1">
-      <c r="A55" s="135" t="n"/>
+      <c r="A55" s="136" t="n"/>
       <c r="B55" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4972,7 +4980,7 @@
         </is>
       </c>
       <c r="D55" s="111" t="n"/>
-      <c r="E55" s="132" t="n">
+      <c r="E55" s="133" t="n">
         <v>13</v>
       </c>
       <c r="F55" s="123" t="n">
@@ -4984,12 +4992,12 @@
       <c r="H55" s="123" t="n">
         <v>56.1737</v>
       </c>
-      <c r="I55" s="133" t="n">
+      <c r="I55" s="134" t="n">
         <v>0.1815</v>
       </c>
     </row>
     <row r="56" ht="27" customHeight="1">
-      <c r="A56" s="135" t="n"/>
+      <c r="A56" s="136" t="n"/>
       <c r="B56" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -4999,7 +5007,7 @@
         </is>
       </c>
       <c r="D56" s="111" t="n"/>
-      <c r="E56" s="132" t="n">
+      <c r="E56" s="133" t="n">
         <v>200</v>
       </c>
       <c r="F56" s="123" t="n">
@@ -5011,12 +5019,12 @@
       <c r="H56" s="123" t="n">
         <v>872</v>
       </c>
-      <c r="I56" s="133" t="n">
+      <c r="I56" s="134" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="135" t="n"/>
+      <c r="A57" s="136" t="n"/>
       <c r="B57" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -5026,7 +5034,7 @@
         </is>
       </c>
       <c r="D57" s="111" t="n"/>
-      <c r="E57" s="132" t="n">
+      <c r="E57" s="133" t="n">
         <v>181</v>
       </c>
       <c r="F57" s="123" t="n">
@@ -5038,12 +5046,12 @@
       <c r="H57" s="123" t="n">
         <v>791.037</v>
       </c>
-      <c r="I57" s="133" t="n">
+      <c r="I57" s="134" t="n">
         <v>2.5409</v>
       </c>
     </row>
     <row r="58" ht="27" customHeight="1">
-      <c r="A58" s="135" t="n"/>
+      <c r="A58" s="136" t="n"/>
       <c r="B58" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -5053,7 +5061,7 @@
         </is>
       </c>
       <c r="D58" s="111" t="n"/>
-      <c r="E58" s="132" t="n">
+      <c r="E58" s="133" t="n">
         <v>8</v>
       </c>
       <c r="F58" s="123" t="n">
@@ -5065,12 +5073,12 @@
       <c r="H58" s="123" t="n">
         <v>34.963</v>
       </c>
-      <c r="I58" s="133" t="n">
+      <c r="I58" s="134" t="n">
         <v>0.1123</v>
       </c>
     </row>
     <row r="59" ht="27" customHeight="1">
-      <c r="A59" s="135" t="n"/>
+      <c r="A59" s="136" t="n"/>
       <c r="B59" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -5080,7 +5088,7 @@
         </is>
       </c>
       <c r="D59" s="111" t="n"/>
-      <c r="E59" s="132" t="n">
+      <c r="E59" s="133" t="n">
         <v>200</v>
       </c>
       <c r="F59" s="123" t="n">
@@ -5092,12 +5100,12 @@
       <c r="H59" s="123" t="n">
         <v>863</v>
       </c>
-      <c r="I59" s="133" t="n">
+      <c r="I59" s="134" t="n">
         <v>2.5344</v>
       </c>
     </row>
     <row r="60" ht="27" customHeight="1">
-      <c r="A60" s="135" t="n"/>
+      <c r="A60" s="136" t="n"/>
       <c r="B60" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -5107,7 +5115,7 @@
         </is>
       </c>
       <c r="D60" s="111" t="n"/>
-      <c r="E60" s="132" t="n">
+      <c r="E60" s="133" t="n">
         <v>200</v>
       </c>
       <c r="F60" s="123" t="n">
@@ -5119,12 +5127,12 @@
       <c r="H60" s="123" t="n">
         <v>827.6596</v>
       </c>
-      <c r="I60" s="133" t="n">
+      <c r="I60" s="134" t="n">
         <v>2.0895</v>
       </c>
     </row>
     <row r="61" ht="27" customHeight="1">
-      <c r="A61" s="135" t="n"/>
+      <c r="A61" s="136" t="n"/>
       <c r="B61" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -5134,7 +5142,7 @@
         </is>
       </c>
       <c r="D61" s="111" t="n"/>
-      <c r="E61" s="132" t="n">
+      <c r="E61" s="133" t="n">
         <v>35</v>
       </c>
       <c r="F61" s="123" t="n">
@@ -5146,12 +5154,12 @@
       <c r="H61" s="123" t="n">
         <v>144.8404</v>
       </c>
-      <c r="I61" s="133" t="n">
+      <c r="I61" s="134" t="n">
         <v>0.3657</v>
       </c>
     </row>
     <row r="62" ht="27" customHeight="1">
-      <c r="A62" s="135" t="n"/>
+      <c r="A62" s="136" t="n"/>
       <c r="B62" s="122" t="n">
         <v>9000688275</v>
       </c>
@@ -5161,7 +5169,7 @@
         </is>
       </c>
       <c r="D62" s="111" t="n"/>
-      <c r="E62" s="132" t="n">
+      <c r="E62" s="133" t="n">
         <v>298</v>
       </c>
       <c r="F62" s="123" t="n">
@@ -5173,24 +5181,24 @@
       <c r="H62" s="123" t="n">
         <v>1275.5</v>
       </c>
-      <c r="I62" s="133" t="n">
+      <c r="I62" s="134" t="n">
         <v>3.2076</v>
       </c>
     </row>
     <row r="63" ht="27" customHeight="1">
-      <c r="A63" s="134" t="n"/>
+      <c r="A63" s="135" t="n"/>
       <c r="B63" s="122" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
         </is>
       </c>
-      <c r="C63" s="129" t="n"/>
-      <c r="D63" s="136" t="n"/>
-      <c r="E63" s="132" t="n"/>
+      <c r="C63" s="130" t="n"/>
+      <c r="D63" s="137" t="n"/>
+      <c r="E63" s="133" t="n"/>
       <c r="F63" s="123" t="n"/>
       <c r="G63" s="123" t="n"/>
       <c r="H63" s="123" t="n"/>
-      <c r="I63" s="133" t="n"/>
+      <c r="I63" s="134" t="n"/>
     </row>
     <row r="64" ht="27" customHeight="1">
       <c r="A64" s="127" t="n"/>
@@ -5205,7 +5213,7 @@
         </is>
       </c>
       <c r="D64" s="111" t="n"/>
-      <c r="E64" s="137">
+      <c r="E64" s="138">
         <f>SUM(E23:E62)</f>
         <v/>
       </c>
@@ -5221,7 +5229,7 @@
         <f>SUM(H23:H62)</f>
         <v/>
       </c>
-      <c r="I64" s="138">
+      <c r="I64" s="139">
         <f>SUM(I23:I62)</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
fixing keybay bug on the price, and descriptoin of good because it has different name from our original code
</commit_message>
<xml_diff>
--- a/invoice_gen/result.xlsx
+++ b/invoice_gen/result.xlsx
@@ -619,6 +619,50 @@
       </bottom>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="00000000"/>
       </left>
@@ -651,50 +695,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border/>
   </borders>
   <cellStyleXfs count="1">
@@ -702,7 +702,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -970,8 +970,8 @@
     <xf numFmtId="0" fontId="27" fillId="3" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1003,7 +1003,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1015,27 +1015,21 @@
     <xf numFmtId="4" fontId="26" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="25" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1048,6 +1042,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="26" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1546,7 +1541,7 @@
       <c r="F8" s="97" t="n"/>
       <c r="G8" s="49" t="inlineStr">
         <is>
-          <t>DAP</t>
+          <t>FOB</t>
         </is>
       </c>
       <c r="H8" s="93" t="n"/>
@@ -1631,7 +1626,8 @@
     <row r="12" ht="22.5" customFormat="1" customHeight="1" s="39">
       <c r="A12" s="103" t="inlineStr">
         <is>
-          <t>1.23.07.0154J</t>
+          <t>1.23.07.0154J/1.23.07.0157J
+1.23.07.0220D</t>
         </is>
       </c>
       <c r="B12" s="101" t="n"/>
@@ -1639,128 +1635,62 @@
       <c r="D12" s="101" t="n"/>
       <c r="E12" s="101" t="n"/>
       <c r="F12" s="102" t="n"/>
-      <c r="G12" s="104" t="n">
-        <v>1.3</v>
+      <c r="G12" s="104">
+        <f>I12/H12</f>
+        <v/>
       </c>
       <c r="H12" s="103" t="n">
-        <v>31925.1</v>
-      </c>
-      <c r="I12" s="104">
-        <f>G12 * H12</f>
-        <v/>
+        <v>123197.8</v>
+      </c>
+      <c r="I12" s="104" t="n">
+        <v>175324.095</v>
       </c>
       <c r="J12" s="102" t="n"/>
     </row>
-    <row r="13" ht="22.5" customFormat="1" customHeight="1" s="39">
-      <c r="A13" s="103" t="inlineStr">
-        <is>
-          <t>1.23.07.0157J</t>
-        </is>
-      </c>
-      <c r="B13" s="101" t="n"/>
+    <row r="13" ht="13.5" customFormat="1" customHeight="1" s="39">
+      <c r="A13" s="105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TOTAL OF: </t>
+        </is>
+      </c>
+      <c r="B13" s="106" t="n"/>
       <c r="C13" s="101" t="n"/>
       <c r="D13" s="101" t="n"/>
       <c r="E13" s="101" t="n"/>
       <c r="F13" s="102" t="n"/>
-      <c r="G13" s="104" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H13" s="103" t="n">
-        <v>11067.7</v>
-      </c>
-      <c r="I13" s="104">
-        <f>G13 * H13</f>
+      <c r="G13" s="107" t="n"/>
+      <c r="H13" s="108">
+        <f>SUM(H12:H12)</f>
         <v/>
       </c>
+      <c r="I13" s="108">
+        <f>SUM(I12:I12)</f>
+        <v/>
+      </c>
       <c r="J13" s="102" t="n"/>
     </row>
-    <row r="14" ht="22.5" customHeight="1" s="88">
-      <c r="A14" s="103" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="B14" s="101" t="n"/>
-      <c r="C14" s="101" t="n"/>
-      <c r="D14" s="101" t="n"/>
-      <c r="E14" s="101" t="n"/>
-      <c r="F14" s="102" t="n"/>
-      <c r="G14" s="104" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="H14" s="103" t="n">
-        <v>78616.8</v>
-      </c>
-      <c r="I14" s="104">
-        <f>G14 * H14</f>
-        <v/>
-      </c>
-      <c r="J14" s="102" t="n"/>
-    </row>
-    <row r="15" ht="22.5" customFormat="1" customHeight="1" s="39">
-      <c r="A15" s="103" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="B15" s="101" t="n"/>
-      <c r="C15" s="101" t="n"/>
-      <c r="D15" s="101" t="n"/>
-      <c r="E15" s="101" t="n"/>
-      <c r="F15" s="102" t="n"/>
-      <c r="G15" s="104" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="H15" s="103" t="n">
-        <v>1588.2</v>
-      </c>
-      <c r="I15" s="104">
-        <f>G15 * H15</f>
-        <v/>
-      </c>
-      <c r="J15" s="102" t="n"/>
-    </row>
-    <row r="16" ht="13.5" customHeight="1" s="88">
-      <c r="A16" s="105" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TOTAL OF: </t>
-        </is>
-      </c>
-      <c r="B16" s="106" t="n"/>
-      <c r="C16" s="101" t="n"/>
-      <c r="D16" s="101" t="n"/>
-      <c r="E16" s="101" t="n"/>
-      <c r="F16" s="102" t="n"/>
-      <c r="G16" s="107" t="n"/>
-      <c r="H16" s="108">
-        <f>SUM(H12:H15)</f>
-        <v/>
-      </c>
-      <c r="I16" s="108">
-        <f>SUM(I12:I15)</f>
-        <v/>
-      </c>
-      <c r="J16" s="102" t="n"/>
-    </row>
+    <row r="14" ht="23.1" customHeight="1" s="88"/>
+    <row r="15" ht="14.1" customFormat="1" customHeight="1" s="39"/>
+    <row r="16" ht="115.5" customHeight="1" s="88"/>
     <row r="17"/>
     <row r="18"/>
     <row r="19" ht="18" customHeight="1" s="88"/>
     <row r="20" ht="18" customHeight="1" s="88"/>
-    <row r="21" ht="18" customHeight="1" s="88"/>
+    <row r="21" ht="18" customHeight="1" s="88">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Authorized Signature For EXporter</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Authorized Signature For Importer</t>
+        </is>
+      </c>
+    </row>
     <row r="22" ht="18" customHeight="1" s="88"/>
     <row r="23" ht="18" customHeight="1" s="88"/>
-    <row r="24" ht="18" customHeight="1" s="88">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Authorized Signature For EXporter</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Authorized Signature For Importer</t>
-        </is>
-      </c>
-    </row>
+    <row r="24" ht="18" customHeight="1" s="88"/>
     <row r="25" ht="18" customHeight="1" s="88"/>
     <row r="26" ht="18" customHeight="1" s="88"/>
     <row r="27" ht="18" customHeight="1" s="88"/>
@@ -1772,35 +1702,20 @@
       <c r="J29" s="112" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="109" t="n"/>
-      <c r="E30" s="110" t="n"/>
-      <c r="F30" s="111" t="n"/>
-      <c r="J30" s="112" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="109" t="n"/>
-      <c r="E31" s="110" t="n"/>
-      <c r="F31" s="111" t="n"/>
-      <c r="J31" s="112" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="109" t="n"/>
-      <c r="E32" s="110" t="n"/>
-      <c r="F32" s="111" t="n"/>
-      <c r="J32" s="112" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="113" t="n"/>
-      <c r="B33" s="114" t="n"/>
-      <c r="C33" s="114" t="n"/>
-      <c r="D33" s="114" t="n"/>
-      <c r="E33" s="115" t="n"/>
-      <c r="F33" s="116" t="n"/>
-      <c r="G33" s="114" t="n"/>
-      <c r="H33" s="114" t="n"/>
-      <c r="I33" s="114" t="n"/>
-      <c r="J33" s="117" t="n"/>
-    </row>
+      <c r="A30" s="113" t="n"/>
+      <c r="B30" s="114" t="n"/>
+      <c r="C30" s="114" t="n"/>
+      <c r="D30" s="114" t="n"/>
+      <c r="E30" s="115" t="n"/>
+      <c r="F30" s="116" t="n"/>
+      <c r="G30" s="114" t="n"/>
+      <c r="H30" s="114" t="n"/>
+      <c r="I30" s="114" t="n"/>
+      <c r="J30" s="117" t="n"/>
+    </row>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
     <row r="34"/>
     <row r="35"/>
     <row r="36"/>
@@ -1969,29 +1884,24 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="35">
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A14:F14"/>
     <mergeCell ref="F4:J4"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A24:E24"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="G1:J1"/>
-    <mergeCell ref="F24:J24"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B13:F13"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A15:F15"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="F19:J19"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A21:E21"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A5:C5"/>
@@ -1999,9 +1909,8 @@
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="I15:J15"/>
     <mergeCell ref="G5:J5"/>
+    <mergeCell ref="F21:J21"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="A19:E19"/>
@@ -2172,7 +2081,7 @@
       <c r="E10" s="10" t="n"/>
       <c r="F10" s="12" t="inlineStr">
         <is>
-          <t>DAP :</t>
+          <t>FOB :</t>
         </is>
       </c>
       <c r="G10" s="16">
@@ -2330,12 +2239,14 @@
       </c>
       <c r="B21" s="121" t="inlineStr">
         <is>
-          <t>RB0604</t>
+          <t>RB0604/RB3358
+SJ0B-317</t>
         </is>
       </c>
       <c r="C21" s="121" t="inlineStr">
         <is>
-          <t>1.23.07.0154J</t>
+          <t>1.23.07.0154J/1.23.07.0157J
+1.23.07.0220D</t>
         </is>
       </c>
       <c r="D21" s="122" t="inlineStr">
@@ -2344,14 +2255,14 @@
         </is>
       </c>
       <c r="E21" s="123" t="n">
-        <v>31925.1</v>
-      </c>
-      <c r="F21" s="123" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="G21" s="124">
-        <f>F21 * E21</f>
+        <v>123197.8</v>
+      </c>
+      <c r="F21" s="123">
+        <f>G21/E21</f>
         <v/>
+      </c>
+      <c r="G21" s="124" t="n">
+        <v>175324.095</v>
       </c>
     </row>
     <row r="22" ht="35" customHeight="1" s="88">
@@ -2360,27 +2271,12 @@
           <t>Des: COW LEATHER</t>
         </is>
       </c>
-      <c r="B22" s="121" t="inlineStr">
-        <is>
-          <t>RB3358</t>
-        </is>
-      </c>
-      <c r="C22" s="121" t="inlineStr">
-        <is>
-          <t>1.23.07.0157J</t>
-        </is>
-      </c>
-      <c r="D22" s="126" t="n"/>
-      <c r="E22" s="123" t="n">
-        <v>11067.7</v>
-      </c>
-      <c r="F22" s="123" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="G22" s="127">
-        <f>F22 * E22</f>
-        <v/>
-      </c>
+      <c r="B22" s="107" t="n"/>
+      <c r="C22" s="107" t="n"/>
+      <c r="D22" s="107" t="n"/>
+      <c r="E22" s="107" t="n"/>
+      <c r="F22" s="107" t="n"/>
+      <c r="G22" s="126" t="n"/>
     </row>
     <row r="23" ht="35" customHeight="1" s="88">
       <c r="A23" s="125" t="inlineStr">
@@ -2388,58 +2284,28 @@
           <t>Case Qty</t>
         </is>
       </c>
-      <c r="B23" s="121" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C23" s="121" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D23" s="126" t="n"/>
-      <c r="E23" s="123" t="n">
-        <v>78616.8</v>
-      </c>
-      <c r="F23" s="123" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="G23" s="127">
-        <f>F23 * E23</f>
-        <v/>
-      </c>
+      <c r="B23" s="107" t="n"/>
+      <c r="C23" s="107" t="n"/>
+      <c r="D23" s="107" t="n"/>
+      <c r="E23" s="107" t="n"/>
+      <c r="F23" s="107" t="n"/>
+      <c r="G23" s="126" t="n"/>
     </row>
     <row r="24" ht="35" customHeight="1" s="88">
-      <c r="A24" s="128" t="inlineStr">
+      <c r="A24" s="127" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
       </c>
-      <c r="B24" s="121" t="inlineStr">
-        <is>
-          <t>SJ0B-317</t>
-        </is>
-      </c>
-      <c r="C24" s="121" t="inlineStr">
-        <is>
-          <t>1.23.07.0220D</t>
-        </is>
-      </c>
-      <c r="D24" s="129" t="n"/>
-      <c r="E24" s="123" t="n">
-        <v>1588.2</v>
-      </c>
-      <c r="F24" s="123" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G24" s="130">
-        <f>F24 * E24</f>
-        <v/>
-      </c>
+      <c r="B24" s="107" t="n"/>
+      <c r="C24" s="107" t="n"/>
+      <c r="D24" s="107" t="n"/>
+      <c r="E24" s="107" t="n"/>
+      <c r="F24" s="107" t="n"/>
+      <c r="G24" s="128" t="n"/>
     </row>
     <row r="25" ht="35" customHeight="1" s="88">
-      <c r="A25" s="131" t="n"/>
+      <c r="A25" s="128" t="n"/>
       <c r="B25" s="119" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL OF: </t>
@@ -2451,7 +2317,7 @@
         </is>
       </c>
       <c r="D25" s="107" t="n"/>
-      <c r="E25" s="132">
+      <c r="E25" s="129">
         <f>SUM(E21:E24)</f>
         <v/>
       </c>
@@ -2733,7 +2599,7 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A1:G1"/>
@@ -2743,9 +2609,8 @@
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D21:D24"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
@@ -2939,7 +2804,7 @@
       <c r="G10" s="5" t="n"/>
       <c r="H10" s="12" t="inlineStr">
         <is>
-          <t>DAP :</t>
+          <t>FOB :</t>
         </is>
       </c>
       <c r="I10" s="16" t="inlineStr">
@@ -3104,10 +2969,10 @@
       </c>
     </row>
     <row r="20" ht="27" customHeight="1" s="88">
-      <c r="A20" s="129" t="n"/>
-      <c r="B20" s="129" t="n"/>
-      <c r="C20" s="129" t="n"/>
-      <c r="D20" s="129" t="n"/>
+      <c r="A20" s="130" t="n"/>
+      <c r="B20" s="130" t="n"/>
+      <c r="C20" s="130" t="n"/>
+      <c r="D20" s="130" t="n"/>
       <c r="E20" s="119" t="inlineStr">
         <is>
           <t>PCS</t>
@@ -3118,12 +2983,12 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G20" s="129" t="n"/>
-      <c r="H20" s="129" t="n"/>
-      <c r="I20" s="129" t="n"/>
+      <c r="G20" s="130" t="n"/>
+      <c r="H20" s="130" t="n"/>
+      <c r="I20" s="130" t="n"/>
     </row>
     <row r="21" ht="27" customHeight="1" s="88">
-      <c r="A21" s="133" t="inlineStr">
+      <c r="A21" s="131" t="inlineStr">
         <is>
           <t>VENDOR#:</t>
         </is>
@@ -3143,7 +3008,7 @@
           <t>COW LEATHER</t>
         </is>
       </c>
-      <c r="E21" s="134" t="n">
+      <c r="E21" s="132" t="n">
         <v>220</v>
       </c>
       <c r="F21" s="123" t="n">
@@ -3155,12 +3020,12 @@
       <c r="H21" s="123" t="n">
         <v>985.5</v>
       </c>
-      <c r="I21" s="135" t="n">
+      <c r="I21" s="133" t="n">
         <v>2.574</v>
       </c>
     </row>
     <row r="22" ht="27" customHeight="1" s="88">
-      <c r="A22" s="136" t="inlineStr">
+      <c r="A22" s="134" t="inlineStr">
         <is>
           <t>Des: LEATHER</t>
         </is>
@@ -3175,8 +3040,8 @@
           <t>1.23.07.0154J</t>
         </is>
       </c>
-      <c r="D22" s="126" t="n"/>
-      <c r="E22" s="134" t="n">
+      <c r="D22" s="135" t="n"/>
+      <c r="E22" s="132" t="n">
         <v>185</v>
       </c>
       <c r="F22" s="123" t="n">
@@ -3188,12 +3053,12 @@
       <c r="H22" s="123" t="n">
         <v>848.5</v>
       </c>
-      <c r="I22" s="135" t="n">
+      <c r="I22" s="133" t="n">
         <v>2.4948</v>
       </c>
     </row>
     <row r="23" ht="27" customHeight="1" s="88">
-      <c r="A23" s="136" t="inlineStr">
+      <c r="A23" s="134" t="inlineStr">
         <is>
           <t>Case Qty</t>
         </is>
@@ -3208,8 +3073,8 @@
           <t>1.23.07.0154J</t>
         </is>
       </c>
-      <c r="D23" s="126" t="n"/>
-      <c r="E23" s="134" t="n">
+      <c r="D23" s="135" t="n"/>
+      <c r="E23" s="132" t="n">
         <v>185</v>
       </c>
       <c r="F23" s="123" t="n">
@@ -3221,12 +3086,12 @@
       <c r="H23" s="123" t="n">
         <v>844.5</v>
       </c>
-      <c r="I23" s="135" t="n">
+      <c r="I23" s="133" t="n">
         <v>2.376</v>
       </c>
     </row>
     <row r="24" ht="27" customHeight="1" s="88">
-      <c r="A24" s="136" t="inlineStr">
+      <c r="A24" s="134" t="inlineStr">
         <is>
           <t>MADE IN CAMBODIA</t>
         </is>
@@ -3241,8 +3106,8 @@
           <t>1.23.07.0157J</t>
         </is>
       </c>
-      <c r="D24" s="126" t="n"/>
-      <c r="E24" s="134" t="n">
+      <c r="D24" s="135" t="n"/>
+      <c r="E24" s="132" t="n">
         <v>190</v>
       </c>
       <c r="F24" s="123" t="n">
@@ -3254,12 +3119,12 @@
       <c r="H24" s="123" t="n">
         <v>888.5</v>
       </c>
-      <c r="I24" s="135" t="n">
+      <c r="I24" s="133" t="n">
         <v>2.97</v>
       </c>
     </row>
     <row r="25" ht="27" customHeight="1" s="88">
-      <c r="A25" s="137" t="n"/>
+      <c r="A25" s="136" t="n"/>
       <c r="B25" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3270,8 +3135,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D25" s="126" t="n"/>
-      <c r="E25" s="134" t="n">
+      <c r="D25" s="135" t="n"/>
+      <c r="E25" s="132" t="n">
         <v>185</v>
       </c>
       <c r="F25" s="123" t="n">
@@ -3283,12 +3148,12 @@
       <c r="H25" s="123" t="n">
         <v>787</v>
       </c>
-      <c r="I25" s="135" t="n">
+      <c r="I25" s="133" t="n">
         <v>2.6532</v>
       </c>
     </row>
     <row r="26" ht="27" customFormat="1" customHeight="1" s="2">
-      <c r="A26" s="137" t="n"/>
+      <c r="A26" s="136" t="n"/>
       <c r="B26" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3299,8 +3164,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D26" s="126" t="n"/>
-      <c r="E26" s="134" t="n">
+      <c r="D26" s="135" t="n"/>
+      <c r="E26" s="132" t="n">
         <v>183</v>
       </c>
       <c r="F26" s="123" t="n">
@@ -3312,12 +3177,12 @@
       <c r="H26" s="123" t="n">
         <v>778.5</v>
       </c>
-      <c r="I26" s="135" t="n">
+      <c r="I26" s="133" t="n">
         <v>2.5344</v>
       </c>
     </row>
     <row r="27" ht="27" customHeight="1" s="88">
-      <c r="A27" s="137" t="n"/>
+      <c r="A27" s="136" t="n"/>
       <c r="B27" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3328,8 +3193,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D27" s="126" t="n"/>
-      <c r="E27" s="134" t="n">
+      <c r="D27" s="135" t="n"/>
+      <c r="E27" s="132" t="n">
         <v>190</v>
       </c>
       <c r="F27" s="123" t="n">
@@ -3341,12 +3206,12 @@
       <c r="H27" s="123" t="n">
         <v>776.5</v>
       </c>
-      <c r="I27" s="135" t="n">
+      <c r="I27" s="133" t="n">
         <v>3.0492</v>
       </c>
     </row>
     <row r="28" ht="27" customHeight="1" s="88">
-      <c r="A28" s="137" t="n"/>
+      <c r="A28" s="136" t="n"/>
       <c r="B28" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3357,8 +3222,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D28" s="126" t="n"/>
-      <c r="E28" s="134" t="n">
+      <c r="D28" s="135" t="n"/>
+      <c r="E28" s="132" t="n">
         <v>190</v>
       </c>
       <c r="F28" s="123" t="n">
@@ -3370,12 +3235,12 @@
       <c r="H28" s="123" t="n">
         <v>774.5</v>
       </c>
-      <c r="I28" s="135" t="n">
+      <c r="I28" s="133" t="n">
         <v>3.0492</v>
       </c>
     </row>
     <row r="29" ht="27" customHeight="1" s="88">
-      <c r="A29" s="137" t="n"/>
+      <c r="A29" s="136" t="n"/>
       <c r="B29" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3386,8 +3251,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D29" s="126" t="n"/>
-      <c r="E29" s="134" t="n">
+      <c r="D29" s="135" t="n"/>
+      <c r="E29" s="132" t="n">
         <v>190</v>
       </c>
       <c r="F29" s="123" t="n">
@@ -3399,12 +3264,12 @@
       <c r="H29" s="123" t="n">
         <v>780</v>
       </c>
-      <c r="I29" s="135" t="n">
+      <c r="I29" s="133" t="n">
         <v>3.0492</v>
       </c>
     </row>
     <row r="30" ht="27" customHeight="1" s="88">
-      <c r="A30" s="137" t="n"/>
+      <c r="A30" s="136" t="n"/>
       <c r="B30" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3415,8 +3280,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D30" s="126" t="n"/>
-      <c r="E30" s="134" t="n">
+      <c r="D30" s="135" t="n"/>
+      <c r="E30" s="132" t="n">
         <v>190</v>
       </c>
       <c r="F30" s="123" t="n">
@@ -3428,12 +3293,12 @@
       <c r="H30" s="123" t="n">
         <v>778</v>
       </c>
-      <c r="I30" s="135" t="n">
+      <c r="I30" s="133" t="n">
         <v>3.0492</v>
       </c>
     </row>
     <row r="31" ht="27" customHeight="1" s="88">
-      <c r="A31" s="137" t="n"/>
+      <c r="A31" s="136" t="n"/>
       <c r="B31" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3444,8 +3309,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D31" s="126" t="n"/>
-      <c r="E31" s="134" t="n">
+      <c r="D31" s="135" t="n"/>
+      <c r="E31" s="132" t="n">
         <v>190</v>
       </c>
       <c r="F31" s="123" t="n">
@@ -3457,12 +3322,12 @@
       <c r="H31" s="123" t="n">
         <v>784</v>
       </c>
-      <c r="I31" s="135" t="n">
+      <c r="I31" s="133" t="n">
         <v>3.0492</v>
       </c>
     </row>
     <row r="32" ht="27" customHeight="1" s="88">
-      <c r="A32" s="137" t="n"/>
+      <c r="A32" s="136" t="n"/>
       <c r="B32" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3473,8 +3338,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D32" s="126" t="n"/>
-      <c r="E32" s="134" t="n">
+      <c r="D32" s="135" t="n"/>
+      <c r="E32" s="132" t="n">
         <v>142</v>
       </c>
       <c r="F32" s="123" t="n">
@@ -3486,12 +3351,12 @@
       <c r="H32" s="123" t="n">
         <v>566.7759</v>
       </c>
-      <c r="I32" s="135" t="n">
+      <c r="I32" s="133" t="n">
         <v>2.4884</v>
       </c>
     </row>
     <row r="33" ht="27" customHeight="1" s="88">
-      <c r="A33" s="137" t="n"/>
+      <c r="A33" s="136" t="n"/>
       <c r="B33" s="121" t="inlineStr">
         <is>
           <t>SJ0B-317</t>
@@ -3502,8 +3367,8 @@
           <t>1.23.07.0220D</t>
         </is>
       </c>
-      <c r="D33" s="129" t="n"/>
-      <c r="E33" s="134" t="n">
+      <c r="D33" s="130" t="n"/>
+      <c r="E33" s="132" t="n">
         <v>32</v>
       </c>
       <c r="F33" s="123" t="n">
@@ -3515,12 +3380,12 @@
       <c r="H33" s="123" t="n">
         <v>127.7241</v>
       </c>
-      <c r="I33" s="135" t="n">
+      <c r="I33" s="133" t="n">
         <v>0.5608</v>
       </c>
     </row>
     <row r="34" ht="27" customHeight="1" s="88">
-      <c r="A34" s="136" t="n"/>
+      <c r="A34" s="134" t="n"/>
       <c r="B34" s="121" t="inlineStr">
         <is>
           <t>LEATHER (HS.CODE: 4107.12.00)</t>
@@ -3528,14 +3393,14 @@
       </c>
       <c r="C34" s="102" t="n"/>
       <c r="D34" s="122" t="n"/>
-      <c r="E34" s="134" t="n"/>
+      <c r="E34" s="132" t="n"/>
       <c r="F34" s="123" t="n"/>
       <c r="G34" s="123" t="n"/>
       <c r="H34" s="123" t="n"/>
-      <c r="I34" s="135" t="n"/>
+      <c r="I34" s="133" t="n"/>
     </row>
     <row r="35" ht="27" customHeight="1" s="88">
-      <c r="A35" s="138" t="n"/>
+      <c r="A35" s="137" t="n"/>
       <c r="B35" s="119" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL OF: </t>
@@ -3547,23 +3412,23 @@
         </is>
       </c>
       <c r="D35" s="107" t="n"/>
-      <c r="E35" s="139">
+      <c r="E35" s="138">
         <f>SUM(E21:E33)</f>
         <v/>
       </c>
-      <c r="F35" s="132">
+      <c r="F35" s="129">
         <f>SUM(F21:F33)</f>
         <v/>
       </c>
-      <c r="G35" s="132">
+      <c r="G35" s="129">
         <f>SUM(G21:G33)</f>
         <v/>
       </c>
-      <c r="H35" s="132">
+      <c r="H35" s="129">
         <f>SUM(H21:H33)</f>
         <v/>
       </c>
-      <c r="I35" s="140">
+      <c r="I35" s="139">
         <f>SUM(I21:I33)</f>
         <v/>
       </c>

</xml_diff>